<commit_message>
Comentar función main y actualizar archivo de salida
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -449,88 +449,28 @@
         <v>folioNc</v>
       </c>
       <c r="P1" t="str">
+        <v>tipoNC</v>
+      </c>
+      <c r="Q1" t="str">
         <v>fechaNc</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="R1" t="str">
         <v>montoDevolucion</v>
       </c>
-      <c r="R1" t="str">
+      <c r="S1" t="str">
         <v>estadoDevolucion</v>
       </c>
-      <c r="S1" t="str">
+      <c r="T1" t="str">
         <v>order</v>
       </c>
-      <c r="T1" t="str">
+      <c r="U1" t="str">
         <v>fechaTicket</v>
-      </c>
-      <c r="U1" t="str">
-        <v>tipoNC</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
         <v>804686</v>
       </c>
-      <c r="B2" t="str">
-        <v>Giovanna Cavagnola</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Jose Miguel Hernandez Cavagnola</v>
-      </c>
-      <c r="D2" t="str">
-        <v>falabella</v>
-      </c>
-      <c r="E2" t="str">
-        <v>051</v>
-      </c>
-      <c r="F2" t="str">
-        <v>19821891989</v>
-      </c>
-      <c r="G2" t="str">
-        <v>763578100</v>
-      </c>
-      <c r="H2" t="str">
-        <v>198929026</v>
-      </c>
-      <c r="I2" t="str">
-        <v>corriente</v>
-      </c>
-      <c r="J2" t="str">
-        <v>cc</v>
-      </c>
-      <c r="K2" t="str">
-        <v>tercero</v>
-      </c>
-      <c r="L2" t="str">
-        <v>3092 Alvi - Pajaritos</v>
-      </c>
-      <c r="M2" t="str">
-        <v>Transferencia</v>
-      </c>
-      <c r="N2" t="str">
-        <v xml:space="preserve">Vuelto Pendiente </v>
-      </c>
-      <c r="O2" t="str">
-        <v>Sin Informacion</v>
-      </c>
-      <c r="P2" t="str">
-        <v>Sin Informacion</v>
-      </c>
-      <c r="Q2" t="str">
-        <v>2</v>
-      </c>
-      <c r="R2" t="str">
-        <v>Devuelto</v>
-      </c>
-      <c r="S2" t="str">
-        <v>589336</v>
-      </c>
-      <c r="T2" t="str">
-        <v>2025-08-21</v>
-      </c>
-      <c r="U2" t="str">
-        <v>Sin Informacion</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -582,19 +522,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q3" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R3" t="str">
         <v>30121</v>
       </c>
-      <c r="R3" t="str">
+      <c r="S3" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S3" t="str">
+      <c r="T3" t="str">
         <v>589092</v>
       </c>
-      <c r="T3" t="str">
+      <c r="U3" t="str">
         <v>2025-08-21</v>
-      </c>
-      <c r="U3" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="4">
@@ -647,19 +587,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q4" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R4" t="str">
         <v>10320</v>
       </c>
-      <c r="R4" t="str">
+      <c r="S4" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S4" t="str">
+      <c r="T4" t="str">
         <v>589203</v>
       </c>
-      <c r="T4" t="str">
+      <c r="U4" t="str">
         <v>2025-08-21</v>
-      </c>
-      <c r="U4" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="5">
@@ -712,19 +652,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q5" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R5" t="str">
         <v>15500</v>
       </c>
-      <c r="R5" t="str">
+      <c r="S5" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S5" t="str">
+      <c r="T5" t="str">
         <v>589211</v>
       </c>
-      <c r="T5" t="str">
+      <c r="U5" t="str">
         <v>2025-08-21</v>
-      </c>
-      <c r="U5" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="6">
@@ -777,19 +717,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q6" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R6" t="str">
         <v>90500</v>
       </c>
-      <c r="R6" t="str">
+      <c r="S6" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S6" t="str">
+      <c r="T6" t="str">
         <v>589073</v>
       </c>
-      <c r="T6" t="str">
+      <c r="U6" t="str">
         <v>2025-08-21</v>
-      </c>
-      <c r="U6" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="7">
@@ -842,19 +782,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q7" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R7" t="str">
         <v>6500</v>
       </c>
-      <c r="R7" t="str">
+      <c r="S7" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S7" t="str">
+      <c r="T7" t="str">
         <v>588833</v>
       </c>
-      <c r="T7" t="str">
+      <c r="U7" t="str">
         <v>2025-08-21</v>
-      </c>
-      <c r="U7" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="8">
@@ -904,22 +844,22 @@
         <v>9642 - 9641 - 9640</v>
       </c>
       <c r="P8" t="str">
+        <v>NC Total</v>
+      </c>
+      <c r="Q8" t="str">
         <v>2025-08-20</v>
       </c>
-      <c r="Q8" t="str">
+      <c r="R8" t="str">
         <v>99255</v>
       </c>
-      <c r="R8" t="str">
+      <c r="S8" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S8" t="str">
+      <c r="T8" t="str">
         <v>589224</v>
       </c>
-      <c r="T8" t="str">
+      <c r="U8" t="str">
         <v>2025-08-19</v>
-      </c>
-      <c r="U8" t="str">
-        <v>NC Total</v>
       </c>
     </row>
     <row r="9">
@@ -969,22 +909,22 @@
         <v>3301</v>
       </c>
       <c r="P9" t="str">
+        <v>NC Parcial</v>
+      </c>
+      <c r="Q9" t="str">
         <v>2025-08-19</v>
       </c>
-      <c r="Q9" t="str">
+      <c r="R9" t="str">
         <v>36700</v>
       </c>
-      <c r="R9" t="str">
+      <c r="S9" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S9" t="str">
+      <c r="T9" t="str">
         <v>588700</v>
       </c>
-      <c r="T9" t="str">
+      <c r="U9" t="str">
         <v>2025-08-13</v>
-      </c>
-      <c r="U9" t="str">
-        <v>NC Parcial</v>
       </c>
     </row>
     <row r="10">
@@ -1037,19 +977,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q10" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R10" t="str">
         <v>3730</v>
       </c>
-      <c r="R10" t="str">
+      <c r="S10" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S10" t="str">
+      <c r="T10" t="str">
         <v>4079252</v>
       </c>
-      <c r="T10" t="str">
+      <c r="U10" t="str">
         <v>2025-08-21</v>
-      </c>
-      <c r="U10" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="11">
@@ -1099,22 +1039,22 @@
         <v>20703627</v>
       </c>
       <c r="P11" t="str">
+        <v>NC Total</v>
+      </c>
+      <c r="Q11" t="str">
         <v>2025-08-20</v>
       </c>
-      <c r="Q11" t="str">
+      <c r="R11" t="str">
         <v>81249</v>
       </c>
-      <c r="R11" t="str">
-        <v>En Proceso MDP</v>
-      </c>
       <c r="S11" t="str">
+        <v>Devuelto</v>
+      </c>
+      <c r="T11" t="str">
         <v>4080562</v>
       </c>
-      <c r="T11" t="str">
+      <c r="U11" t="str">
         <v>2025-08-20</v>
-      </c>
-      <c r="U11" t="str">
-        <v>NC Total</v>
       </c>
     </row>
     <row r="12">
@@ -1164,22 +1104,22 @@
         <v>20689415 - 20689414</v>
       </c>
       <c r="P12" t="str">
+        <v>NC Total</v>
+      </c>
+      <c r="Q12" t="str">
         <v>2025-08-20</v>
       </c>
-      <c r="Q12" t="str">
+      <c r="R12" t="str">
         <v>99331</v>
       </c>
-      <c r="R12" t="str">
+      <c r="S12" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S12" t="str">
+      <c r="T12" t="str">
         <v>4080135</v>
       </c>
-      <c r="T12" t="str">
+      <c r="U12" t="str">
         <v>2025-08-19</v>
-      </c>
-      <c r="U12" t="str">
-        <v>NC Total</v>
       </c>
     </row>
     <row r="13">
@@ -1229,22 +1169,22 @@
         <v>20695553</v>
       </c>
       <c r="P13" t="str">
+        <v>NC Total</v>
+      </c>
+      <c r="Q13" t="str">
         <v>2025-08-20</v>
       </c>
-      <c r="Q13" t="str">
+      <c r="R13" t="str">
         <v>17736</v>
       </c>
-      <c r="R13" t="str">
+      <c r="S13" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S13" t="str">
+      <c r="T13" t="str">
         <v>4079320</v>
       </c>
-      <c r="T13" t="str">
+      <c r="U13" t="str">
         <v>2025-08-19</v>
-      </c>
-      <c r="U13" t="str">
-        <v>NC Total</v>
       </c>
     </row>
     <row r="14">
@@ -1294,22 +1234,22 @@
         <v>20689413</v>
       </c>
       <c r="P14" t="str">
+        <v>NC Parcial</v>
+      </c>
+      <c r="Q14" t="str">
         <v>2025-08-20</v>
       </c>
-      <c r="Q14" t="str">
+      <c r="R14" t="str">
         <v>4020</v>
       </c>
-      <c r="R14" t="str">
+      <c r="S14" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S14" t="str">
+      <c r="T14" t="str">
         <v>4079358</v>
       </c>
-      <c r="T14" t="str">
+      <c r="U14" t="str">
         <v>2025-08-19</v>
-      </c>
-      <c r="U14" t="str">
-        <v>NC Parcial</v>
       </c>
     </row>
     <row r="15">
@@ -1359,22 +1299,22 @@
         <v>20704001</v>
       </c>
       <c r="P15" t="str">
+        <v>NC Total</v>
+      </c>
+      <c r="Q15" t="str">
         <v>2025-08-19</v>
       </c>
-      <c r="Q15" t="str">
+      <c r="R15" t="str">
         <v>25544</v>
       </c>
-      <c r="R15" t="str">
+      <c r="S15" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S15" t="str">
+      <c r="T15" t="str">
         <v>4078605</v>
       </c>
-      <c r="T15" t="str">
+      <c r="U15" t="str">
         <v>2025-08-18</v>
-      </c>
-      <c r="U15" t="str">
-        <v>NC Total</v>
       </c>
     </row>
     <row r="16">
@@ -1424,22 +1364,22 @@
         <v>20701931</v>
       </c>
       <c r="P16" t="str">
+        <v>NC Total</v>
+      </c>
+      <c r="Q16" t="str">
         <v>2025-08-18</v>
       </c>
-      <c r="Q16" t="str">
+      <c r="R16" t="str">
         <v>55875</v>
       </c>
-      <c r="R16" t="str">
-        <v>En Proceso MDP</v>
-      </c>
       <c r="S16" t="str">
+        <v>Devuelto</v>
+      </c>
+      <c r="T16" t="str">
         <v>4076675</v>
       </c>
-      <c r="T16" t="str">
+      <c r="U16" t="str">
         <v>2025-08-18</v>
-      </c>
-      <c r="U16" t="str">
-        <v>NC Total</v>
       </c>
     </row>
     <row r="17">
@@ -1489,22 +1429,22 @@
         <v>20705443</v>
       </c>
       <c r="P17" t="str">
+        <v>NC Total</v>
+      </c>
+      <c r="Q17" t="str">
         <v>2025-08-19</v>
       </c>
-      <c r="Q17" t="str">
+      <c r="R17" t="str">
         <v>142780</v>
       </c>
-      <c r="R17" t="str">
+      <c r="S17" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S17" t="str">
+      <c r="T17" t="str">
         <v>4078003</v>
       </c>
-      <c r="T17" t="str">
+      <c r="U17" t="str">
         <v>2025-08-18</v>
-      </c>
-      <c r="U17" t="str">
-        <v>NC Total</v>
       </c>
     </row>
     <row r="18">
@@ -1557,19 +1497,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q18" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R18" t="str">
         <v>2429</v>
       </c>
-      <c r="R18" t="str">
+      <c r="S18" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S18" t="str">
+      <c r="T18" t="str">
         <v>4076915</v>
       </c>
-      <c r="T18" t="str">
+      <c r="U18" t="str">
         <v>2025-08-18</v>
-      </c>
-      <c r="U18" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="19">
@@ -1622,19 +1562,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q19" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R19" t="str">
         <v>10054</v>
       </c>
-      <c r="R19" t="str">
+      <c r="S19" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S19" t="str">
+      <c r="T19" t="str">
         <v>4076219</v>
       </c>
-      <c r="T19" t="str">
+      <c r="U19" t="str">
         <v>2025-08-18</v>
-      </c>
-      <c r="U19" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="20">
@@ -1687,19 +1627,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q20" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R20" t="str">
         <v>1124</v>
       </c>
-      <c r="R20" t="str">
+      <c r="S20" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S20" t="str">
+      <c r="T20" t="str">
         <v>4076149</v>
       </c>
-      <c r="T20" t="str">
+      <c r="U20" t="str">
         <v>2025-08-18</v>
-      </c>
-      <c r="U20" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="21">
@@ -1752,19 +1692,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q21" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R21" t="str">
         <v>12358</v>
       </c>
-      <c r="R21" t="str">
+      <c r="S21" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S21" t="str">
+      <c r="T21" t="str">
         <v>4074870</v>
       </c>
-      <c r="T21" t="str">
+      <c r="U21" t="str">
         <v>2025-08-18</v>
-      </c>
-      <c r="U21" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="22">
@@ -1817,19 +1757,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q22" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R22" t="str">
         <v>4260</v>
       </c>
-      <c r="R22" t="str">
+      <c r="S22" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S22" t="str">
+      <c r="T22" t="str">
         <v>4073675</v>
       </c>
-      <c r="T22" t="str">
+      <c r="U22" t="str">
         <v>2025-08-18</v>
-      </c>
-      <c r="U22" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="23">
@@ -1882,19 +1822,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q23" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R23" t="str">
         <v>3745</v>
       </c>
-      <c r="R23" t="str">
+      <c r="S23" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S23" t="str">
+      <c r="T23" t="str">
         <v>4072924</v>
       </c>
-      <c r="T23" t="str">
+      <c r="U23" t="str">
         <v>2025-08-18</v>
-      </c>
-      <c r="U23" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="24">
@@ -1947,19 +1887,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q24" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R24" t="str">
         <v>3626</v>
       </c>
-      <c r="R24" t="str">
+      <c r="S24" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S24" t="str">
+      <c r="T24" t="str">
         <v>4070820</v>
       </c>
-      <c r="T24" t="str">
+      <c r="U24" t="str">
         <v>2025-08-18</v>
-      </c>
-      <c r="U24" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="25">
@@ -2009,22 +1949,22 @@
         <v>20706892 - 20705444</v>
       </c>
       <c r="P25" t="str">
+        <v>NC Total</v>
+      </c>
+      <c r="Q25" t="str">
         <v>2025-08-19</v>
       </c>
-      <c r="Q25" t="str">
+      <c r="R25" t="str">
         <v>127860</v>
       </c>
-      <c r="R25" t="str">
+      <c r="S25" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S25" t="str">
+      <c r="T25" t="str">
         <v>4077919</v>
       </c>
-      <c r="T25" t="str">
+      <c r="U25" t="str">
         <v>2025-08-18</v>
-      </c>
-      <c r="U25" t="str">
-        <v>NC Total</v>
       </c>
     </row>
     <row r="26">
@@ -2074,22 +2014,22 @@
         <v>20698819-20698818</v>
       </c>
       <c r="P26" t="str">
+        <v>NC Total</v>
+      </c>
+      <c r="Q26" t="str">
         <v>2025-08-18</v>
       </c>
-      <c r="Q26" t="str">
+      <c r="R26" t="str">
         <v>71676</v>
       </c>
-      <c r="R26" t="str">
+      <c r="S26" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S26" t="str">
+      <c r="T26" t="str">
         <v>4077729</v>
       </c>
-      <c r="T26" t="str">
+      <c r="U26" t="str">
         <v>2025-08-17</v>
-      </c>
-      <c r="U26" t="str">
-        <v>NC Total</v>
       </c>
     </row>
     <row r="27">
@@ -2139,22 +2079,22 @@
         <v>20706653</v>
       </c>
       <c r="P27" t="str">
+        <v>NC Total</v>
+      </c>
+      <c r="Q27" t="str">
         <v>2025-08-18</v>
       </c>
-      <c r="Q27" t="str">
+      <c r="R27" t="str">
         <v>34648</v>
       </c>
-      <c r="R27" t="str">
+      <c r="S27" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S27" t="str">
+      <c r="T27" t="str">
         <v>4075141</v>
       </c>
-      <c r="T27" t="str">
+      <c r="U27" t="str">
         <v>2025-08-17</v>
-      </c>
-      <c r="U27" t="str">
-        <v>NC Total</v>
       </c>
     </row>
     <row r="28">
@@ -2204,22 +2144,22 @@
         <v>20692764</v>
       </c>
       <c r="P28" t="str">
+        <v>NC Parcial</v>
+      </c>
+      <c r="Q28" t="str">
         <v>2025-08-18</v>
       </c>
-      <c r="Q28" t="str">
+      <c r="R28" t="str">
         <v>1590</v>
       </c>
-      <c r="R28" t="str">
+      <c r="S28" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S28" t="str">
+      <c r="T28" t="str">
         <v>4076325</v>
       </c>
-      <c r="T28" t="str">
+      <c r="U28" t="str">
         <v>2025-08-16</v>
-      </c>
-      <c r="U28" t="str">
-        <v>NC Parcial</v>
       </c>
     </row>
     <row r="29">
@@ -2269,22 +2209,22 @@
         <v>20697957</v>
       </c>
       <c r="P29" t="str">
+        <v>NC Parcial</v>
+      </c>
+      <c r="Q29" t="str">
         <v>2025-08-18</v>
       </c>
-      <c r="Q29" t="str">
+      <c r="R29" t="str">
         <v>1096</v>
       </c>
-      <c r="R29" t="str">
+      <c r="S29" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S29" t="str">
+      <c r="T29" t="str">
         <v>4075375</v>
       </c>
-      <c r="T29" t="str">
+      <c r="U29" t="str">
         <v>2025-08-16</v>
-      </c>
-      <c r="U29" t="str">
-        <v>NC Parcial</v>
       </c>
     </row>
     <row r="30">
@@ -2334,22 +2274,22 @@
         <v>20702879</v>
       </c>
       <c r="P30" t="str">
+        <v>NC Parcial</v>
+      </c>
+      <c r="Q30" t="str">
         <v>2025-08-18</v>
       </c>
-      <c r="Q30" t="str">
+      <c r="R30" t="str">
         <v>3845</v>
       </c>
-      <c r="R30" t="str">
+      <c r="S30" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S30" t="str">
+      <c r="T30" t="str">
         <v>4074458</v>
       </c>
-      <c r="T30" t="str">
+      <c r="U30" t="str">
         <v>2025-08-15</v>
-      </c>
-      <c r="U30" t="str">
-        <v>NC Parcial</v>
       </c>
     </row>
     <row r="31">
@@ -2399,22 +2339,22 @@
         <v>20697956</v>
       </c>
       <c r="P31" t="str">
+        <v>NC Parcial</v>
+      </c>
+      <c r="Q31" t="str">
         <v>2025-08-17</v>
       </c>
-      <c r="Q31" t="str">
+      <c r="R31" t="str">
         <v>5764</v>
       </c>
-      <c r="R31" t="str">
+      <c r="S31" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S31" t="str">
+      <c r="T31" t="str">
         <v>4072782</v>
       </c>
-      <c r="T31" t="str">
+      <c r="U31" t="str">
         <v>2025-08-15</v>
-      </c>
-      <c r="U31" t="str">
-        <v>NC Parcial</v>
       </c>
     </row>
     <row r="32">
@@ -2464,22 +2404,22 @@
         <v>20645671-20645672- 20645670</v>
       </c>
       <c r="P32" t="str">
+        <v>NC Total</v>
+      </c>
+      <c r="Q32" t="str">
         <v>2025-08-18</v>
       </c>
-      <c r="Q32" t="str">
+      <c r="R32" t="str">
         <v>84477</v>
       </c>
-      <c r="R32" t="str">
+      <c r="S32" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S32" t="str">
+      <c r="T32" t="str">
         <v>4070707</v>
       </c>
-      <c r="T32" t="str">
+      <c r="U32" t="str">
         <v>2025-08-14</v>
-      </c>
-      <c r="U32" t="str">
-        <v>NC Total</v>
       </c>
     </row>
     <row r="33">
@@ -2529,22 +2469,22 @@
         <v>20699532</v>
       </c>
       <c r="P33" t="str">
+        <v>NC Parcial</v>
+      </c>
+      <c r="Q33" t="str">
         <v>2025-08-14</v>
       </c>
-      <c r="Q33" t="str">
+      <c r="R33" t="str">
         <v>3894</v>
       </c>
-      <c r="R33" t="str">
+      <c r="S33" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S33" t="str">
+      <c r="T33" t="str">
         <v>4068171</v>
       </c>
-      <c r="T33" t="str">
+      <c r="U33" t="str">
         <v>2025-08-12</v>
-      </c>
-      <c r="U33" t="str">
-        <v>NC Parcial</v>
       </c>
     </row>
     <row r="34">
@@ -2597,19 +2537,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q34" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R34" t="str">
         <v>16474</v>
       </c>
-      <c r="R34" t="str">
+      <c r="S34" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S34" t="str">
+      <c r="T34" t="str">
         <v>4079861</v>
       </c>
-      <c r="T34" t="str">
+      <c r="U34" t="str">
         <v>2025-08-21</v>
-      </c>
-      <c r="U34" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="35">
@@ -2662,19 +2602,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q35" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R35" t="str">
         <v>8896</v>
       </c>
-      <c r="R35" t="str">
+      <c r="S35" t="str">
         <v>Sin Datos Bancarios</v>
       </c>
-      <c r="S35" t="str">
+      <c r="T35" t="str">
         <v>4079098</v>
       </c>
-      <c r="T35" t="str">
+      <c r="U35" t="str">
         <v>2025-08-21</v>
-      </c>
-      <c r="U35" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="36">
@@ -2727,19 +2667,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q36" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R36" t="str">
         <v>590</v>
       </c>
-      <c r="R36" t="str">
+      <c r="S36" t="str">
         <v>Devuelto</v>
       </c>
-      <c r="S36" t="str">
+      <c r="T36" t="str">
         <v>4078692</v>
       </c>
-      <c r="T36" t="str">
+      <c r="U36" t="str">
         <v>2025-08-21</v>
-      </c>
-      <c r="U36" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="37">
@@ -2792,19 +2732,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q37" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R37" t="str">
         <v>4194</v>
       </c>
-      <c r="R37" t="str">
+      <c r="S37" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S37" t="str">
+      <c r="T37" t="str">
         <v>4077921</v>
       </c>
-      <c r="T37" t="str">
+      <c r="U37" t="str">
         <v>2025-08-21</v>
-      </c>
-      <c r="U37" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="38">
@@ -2857,19 +2797,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q38" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R38" t="str">
         <v>4218</v>
       </c>
-      <c r="R38" t="str">
+      <c r="S38" t="str">
         <v>Sin Datos Bancarios</v>
       </c>
-      <c r="S38" t="str">
+      <c r="T38" t="str">
         <v>4077245</v>
       </c>
-      <c r="T38" t="str">
+      <c r="U38" t="str">
         <v>2025-08-21</v>
-      </c>
-      <c r="U38" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="39">
@@ -2922,19 +2862,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q39" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R39" t="str">
         <v>4407</v>
       </c>
-      <c r="R39" t="str">
+      <c r="S39" t="str">
         <v>Pendiente</v>
       </c>
-      <c r="S39" t="str">
+      <c r="T39" t="str">
         <v>4077835</v>
       </c>
-      <c r="T39" t="str">
+      <c r="U39" t="str">
         <v>2025-08-18</v>
-      </c>
-      <c r="U39" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="40">
@@ -2987,19 +2927,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q40" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R40" t="str">
         <v>3734</v>
       </c>
-      <c r="R40" t="str">
+      <c r="S40" t="str">
         <v>Sin Datos Bancarios</v>
       </c>
-      <c r="S40" t="str">
+      <c r="T40" t="str">
         <v>4075725</v>
       </c>
-      <c r="T40" t="str">
+      <c r="U40" t="str">
         <v>2025-08-18</v>
-      </c>
-      <c r="U40" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="41">
@@ -3052,19 +2992,19 @@
         <v>Sin Informacion</v>
       </c>
       <c r="Q41" t="str">
+        <v>Sin Informacion</v>
+      </c>
+      <c r="R41" t="str">
         <v>4928</v>
       </c>
-      <c r="R41" t="str">
+      <c r="S41" t="str">
         <v>Sin Datos Bancarios</v>
       </c>
-      <c r="S41" t="str">
+      <c r="T41" t="str">
         <v>4075119</v>
       </c>
-      <c r="T41" t="str">
+      <c r="U41" t="str">
         <v>2025-08-18</v>
-      </c>
-      <c r="U41" t="str">
-        <v>Sin Informacion</v>
       </c>
     </row>
     <row r="42">
@@ -3114,22 +3054,22 @@
         <v>20703330</v>
       </c>
       <c r="P42" t="str">
+        <v>NC Parcial</v>
+      </c>
+      <c r="Q42" t="str">
         <v>2025-08-19</v>
       </c>
-      <c r="Q42" t="str">
+      <c r="R42" t="str">
         <v>3097</v>
       </c>
-      <c r="R42" t="str">
+      <c r="S42" t="str">
         <v>Sin Datos Bancarios</v>
       </c>
-      <c r="S42" t="str">
+      <c r="T42" t="str">
         <v>4077787</v>
       </c>
-      <c r="T42" t="str">
+      <c r="U42" t="str">
         <v>2025-08-17</v>
-      </c>
-      <c r="U42" t="str">
-        <v>NC Parcial</v>
       </c>
     </row>
     <row r="43">
@@ -3179,22 +3119,22 @@
         <v>20704068</v>
       </c>
       <c r="P43" t="str">
+        <v>NC Parcial</v>
+      </c>
+      <c r="Q43" t="str">
         <v>2025-08-18</v>
       </c>
-      <c r="Q43" t="str">
+      <c r="R43" t="str">
         <v>1476</v>
       </c>
-      <c r="R43" t="str">
+      <c r="S43" t="str">
         <v>Sin Datos Bancarios</v>
       </c>
-      <c r="S43" t="str">
+      <c r="T43" t="str">
         <v>4074592</v>
       </c>
-      <c r="T43" t="str">
+      <c r="U43" t="str">
         <v>2025-08-17</v>
-      </c>
-      <c r="U43" t="str">
-        <v>NC Parcial</v>
       </c>
     </row>
     <row r="44">
@@ -3244,22 +3184,22 @@
         <v>20701671</v>
       </c>
       <c r="P44" t="str">
+        <v>NC Parcial</v>
+      </c>
+      <c r="Q44" t="str">
         <v>2025-08-15</v>
       </c>
-      <c r="Q44" t="str">
+      <c r="R44" t="str">
         <v>16580</v>
       </c>
-      <c r="R44" t="str">
+      <c r="S44" t="str">
         <v>Sin Datos Bancarios</v>
       </c>
-      <c r="S44" t="str">
+      <c r="T44" t="str">
         <v>4071929</v>
       </c>
-      <c r="T44" t="str">
+      <c r="U44" t="str">
         <v>2025-08-14</v>
-      </c>
-      <c r="U44" t="str">
-        <v>NC Parcial</v>
       </c>
     </row>
     <row r="45">
@@ -3309,22 +3249,22 @@
         <v>6385</v>
       </c>
       <c r="P45" t="str">
+        <v>NC Parcial</v>
+      </c>
+      <c r="Q45" t="str">
         <v>2025-08-14</v>
       </c>
-      <c r="Q45" t="str">
+      <c r="R45" t="str">
         <v>1030</v>
       </c>
-      <c r="R45" t="str">
+      <c r="S45" t="str">
         <v>Sin Datos Bancarios</v>
       </c>
-      <c r="S45" t="str">
+      <c r="T45" t="str">
         <v>588606</v>
       </c>
-      <c r="T45" t="str">
+      <c r="U45" t="str">
         <v>2025-08-13</v>
-      </c>
-      <c r="U45" t="str">
-        <v>NC Parcial</v>
       </c>
     </row>
     <row r="46">
@@ -3374,22 +3314,22 @@
         <v>8249</v>
       </c>
       <c r="P46" t="str">
+        <v>NC Parcial</v>
+      </c>
+      <c r="Q46" t="str">
         <v>2025-08-14</v>
       </c>
-      <c r="Q46" t="str">
+      <c r="R46" t="str">
         <v>4860</v>
       </c>
-      <c r="R46" t="str">
+      <c r="S46" t="str">
         <v>Sin Datos Bancarios</v>
       </c>
-      <c r="S46" t="str">
+      <c r="T46" t="str">
         <v>588497</v>
       </c>
-      <c r="T46" t="str">
+      <c r="U46" t="str">
         <v>2025-08-12</v>
-      </c>
-      <c r="U46" t="str">
-        <v>NC Parcial</v>
       </c>
     </row>
   </sheetData>

</xml_diff>